<commit_message>
initial implementation of import workig, needs cleanup and validations
</commit_message>
<xml_diff>
--- a/TravelEditor/Data/exported_data.xlsx
+++ b/TravelEditor/Data/exported_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>TripId</t>
   </si>
@@ -55,190 +55,199 @@
     <t>probno putovanje</t>
   </si>
   <si>
-    <t>Paris, France</t>
+    <t>{"DestinationId":1,"City":"Paris","Country":"France"}</t>
+  </si>
+  <si>
+    <t>[{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
+  </si>
+  <si>
+    <t>[{"ReviewId":11,"Comment":"aq","Rating":10}]</t>
+  </si>
+  <si>
+    <t>putovanje2</t>
+  </si>
+  <si>
+    <t>neki opisss</t>
+  </si>
+  <si>
+    <t>{"DestinationId":5,"City":"nova Destinacija","Country":"novann"}</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>DestinationId</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Attractions</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>The capital city of France, known for its art, fashion, and culture.</t>
+  </si>
+  <si>
+    <t>Cold,</t>
+  </si>
+  <si>
+    <t>[{"AttractionId":3,"Name":"Notre Dame Cathedral"},{"AttractionId":4,"Name":"Montmartre"}]</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>The largest city in the United States, known for its skyline and cultural diversity.</t>
+  </si>
+  <si>
+    <t>Humid subtropical</t>
+  </si>
+  <si>
+    <t>[{"AttractionId":2,"Name":"Central Park"},{"AttractionId":32,"Name":"Statue of Libertyy"}]</t>
+  </si>
+  <si>
+    <t>nova Destinacija</t>
+  </si>
+  <si>
+    <t>novann</t>
+  </si>
+  <si>
+    <t>nova</t>
+  </si>
+  <si>
+    <t>novaaa</t>
+  </si>
+  <si>
+    <t>AttractionId</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Central Park</t>
+  </si>
+  <si>
+    <t>A large public park in New York City, designed by Frederick Law Olmsted and Calvert Vaux.</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
+  </si>
+  <si>
+    <t>Notre Dame Cathedral</t>
+  </si>
+  <si>
+    <t>A medieval Catholic cathedral, considered one of the finest examples of French Gothic architecture.</t>
+  </si>
+  <si>
+    <t>6 Parvis Notre-Dame - Pl. Jean-Paul II, 75004 Paris, France</t>
+  </si>
+  <si>
+    <t>Montmartre</t>
+  </si>
+  <si>
+    <t>A large hill in Paris known for its artistic history and the Basilica of the Sacré-Cœur.</t>
+  </si>
+  <si>
+    <t>18th Arrondissement, Paris, France</t>
+  </si>
+  <si>
+    <t>Statue of Libertyy</t>
+  </si>
+  <si>
+    <t>A colossal neoclassical sculpture on Liberty Island in New York City.</t>
+  </si>
+  <si>
+    <t>Liberty Island, New York</t>
+  </si>
+  <si>
+    <t>TravellerId</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>mika</t>
+  </si>
+  <si>
+    <t>mikic</t>
   </si>
   <si>
     <t>mika@gmail.com</t>
   </si>
   <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>pera</t>
+  </si>
+  <si>
+    <t>peric</t>
+  </si>
+  <si>
+    <t>pera@gmail.com</t>
+  </si>
+  <si>
+    <t>jedan</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>ReviewId</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Traveller</t>
+  </si>
+  <si>
     <t>aq</t>
   </si>
   <si>
-    <t>putovanje2</t>
-  </si>
-  <si>
-    <t>neki opisss</t>
-  </si>
-  <si>
-    <t>nova Destinacija, novann</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>DestinationId</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Climate</t>
-  </si>
-  <si>
-    <t>Attractions</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>The capital city of France, known for its art, fashion, and culture.</t>
-  </si>
-  <si>
-    <t>Cold,</t>
-  </si>
-  <si>
-    <t>Notre Dame Cathedral, Montmartre</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>The largest city in the United States, known for its skyline and cultural diversity.</t>
-  </si>
-  <si>
-    <t>Humid subtropical</t>
-  </si>
-  <si>
-    <t>Central Park, Statue of Libertyy</t>
-  </si>
-  <si>
-    <t>nova Destinacija</t>
-  </si>
-  <si>
-    <t>novann</t>
-  </si>
-  <si>
-    <t>nova</t>
-  </si>
-  <si>
-    <t>novaaa</t>
-  </si>
-  <si>
-    <t>AttractionId</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Central Park</t>
-  </si>
-  <si>
-    <t>A large public park in New York City, designed by Frederick Law Olmsted and Calvert Vaux.</t>
-  </si>
-  <si>
-    <t>New York, NY</t>
-  </si>
-  <si>
-    <t>Notre Dame Cathedral</t>
-  </si>
-  <si>
-    <t>A medieval Catholic cathedral, considered one of the finest examples of French Gothic architecture.</t>
-  </si>
-  <si>
-    <t>6 Parvis Notre-Dame - Pl. Jean-Paul II, 75004 Paris, France</t>
-  </si>
-  <si>
-    <t>Montmartre</t>
-  </si>
-  <si>
-    <t>A large hill in Paris known for its artistic history and the Basilica of the Sacré-Cœur.</t>
-  </si>
-  <si>
-    <t>18th Arrondissement, Paris, France</t>
-  </si>
-  <si>
-    <t>Statue of Libertyy</t>
-  </si>
-  <si>
-    <t>A colossal neoclassical sculpture on Liberty Island in New York City.</t>
-  </si>
-  <si>
-    <t>Liberty Island, New York</t>
-  </si>
-  <si>
-    <t>TravellerId</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>mika</t>
-  </si>
-  <si>
-    <t>mikic</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>pera</t>
-  </si>
-  <si>
-    <t>peric</t>
-  </si>
-  <si>
-    <t>pera@gmail.com</t>
-  </si>
-  <si>
-    <t>jedan</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>ReviewId</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Traveller</t>
+    <t>{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}</t>
   </si>
   <si>
     <t>Spire.XLS for .NET</t>
@@ -758,9 +767,9 @@
     <col min="2" max="2" width="10.00390625" widthPt="52.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" widthPt="79.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.57421875" widthPt="113.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.00390625" widthPt="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.00390625" widthPt="278.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.421875" widthPt="285.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.57421875" widthPt="202.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75">
@@ -834,6 +843,12 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="12.75">
       <c r="A4">
@@ -853,6 +868,12 @@
       </c>
       <c r="F4" t="s">
         <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -875,7 +896,7 @@
     <col min="3" max="3" width="7.7109375" widthPt="40.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.00390625" widthPt="351.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" widthPt="84.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" widthPt="158.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.57421875" widthPt="396.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
@@ -953,6 +974,9 @@
       </c>
       <c r="E4" t="s">
         <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1116,10 +1140,10 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <v>34</v>
@@ -1130,16 +1154,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
       </c>
       <c r="F3">
         <v>19</v>
@@ -1150,16 +1174,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -1185,27 +1209,27 @@
     <col min="3" max="3" width="6.57421875" widthPt="34.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" widthPt="82.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.28125" widthPt="279.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
         <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
@@ -1213,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1225,7 +1249,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1245,42 +1269,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing import logic to be more generic and cleaner
</commit_message>
<xml_diff>
--- a/TravelEditor/Data/exported_data.xlsx
+++ b/TravelEditor/Data/exported_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>TripId</t>
   </si>
@@ -55,13 +55,13 @@
     <t>probno putovanje</t>
   </si>
   <si>
-    <t>{"DestinationId":1,"City":"Paris","Country":"France"}</t>
-  </si>
-  <si>
-    <t>[{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
-  </si>
-  <si>
-    <t>[{"ReviewId":11,"Comment":"aq","Rating":10}]</t>
+    <t>{"DestinationId":60,"City":"Paris","Country":"France"}</t>
+  </si>
+  <si>
+    <t>[{"TravellerId":63,"Email":"mika@gmail.com","FirstName":"mika"}]</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
   <si>
     <t>putovanje2</t>
@@ -70,10 +70,7 @@
     <t>neki opisss</t>
   </si>
   <si>
-    <t>{"DestinationId":5,"City":"nova Destinacija","Country":"novann"}</t>
-  </si>
-  <si>
-    <t>[]</t>
+    <t>{"DestinationId":62,"City":"nova Destinacija","Country":"novann"}</t>
   </si>
   <si>
     <t>w</t>
@@ -109,7 +106,7 @@
     <t>Cold,</t>
   </si>
   <si>
-    <t>[{"AttractionId":3,"Name":"Notre Dame Cathedral"},{"AttractionId":4,"Name":"Montmartre"}]</t>
+    <t>[{"AttractionId":96,"Name":"Notre Dame Cathedral"},{"AttractionId":97,"Name":"Montmartre"}]</t>
   </si>
   <si>
     <t>New York</t>
@@ -124,7 +121,7 @@
     <t>Humid subtropical</t>
   </si>
   <si>
-    <t>[{"AttractionId":2,"Name":"Central Park"},{"AttractionId":32,"Name":"Statue of Libertyy"}]</t>
+    <t>[{"AttractionId":98,"Name":"Statue of Libertyy"}]</t>
   </si>
   <si>
     <t>nova Destinacija</t>
@@ -148,15 +145,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Central Park</t>
-  </si>
-  <si>
-    <t>A large public park in New York City, designed by Frederick Law Olmsted and Calvert Vaux.</t>
-  </si>
-  <si>
-    <t>New York, NY</t>
-  </si>
-  <si>
     <t>Notre Dame Cathedral</t>
   </si>
   <si>
@@ -227,27 +215,6 @@
   </si>
   <si>
     <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>ReviewId</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Rating</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Traveller</t>
-  </si>
-  <si>
-    <t>aq</t>
-  </si>
-  <si>
-    <t>{"TravellerId":3,"Email":"mika@gmail.com","FirstName":"mika"}</t>
   </si>
   <si>
     <t>Spire.XLS for .NET</t>
@@ -767,9 +734,9 @@
     <col min="2" max="2" width="10.00390625" widthPt="52.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" widthPt="79.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.00390625" widthPt="278.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.421875" widthPt="285.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.57421875" widthPt="202.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.00390625" widthPt="283.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.421875" widthPt="291" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.00390625" widthPt="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75">
@@ -800,7 +767,7 @@
     </row>
     <row r="2" spans="1:8" ht="12.75">
       <c r="A2">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -826,7 +793,7 @@
     </row>
     <row r="3" spans="1:8" ht="12.75">
       <c r="A3">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -844,18 +811,18 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75">
       <c r="A4">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>45870</v>
@@ -864,16 +831,16 @@
         <v>45879</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -896,87 +863,87 @@
     <col min="3" max="3" width="7.7109375" widthPt="40.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.00390625" widthPt="351.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" widthPt="84.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.57421875" widthPt="396.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.57421875" widthPt="407.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
       <c r="A2">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75">
       <c r="A3">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
       <c r="A4">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -988,7 +955,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -1003,7 +970,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1012,78 +979,61 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75">
       <c r="A2">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75">
       <c r="A3">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>45</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75">
       <c r="A4">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75">
-      <c r="A5">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1111,39 +1061,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
       <c r="A2">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F2">
         <v>34</v>
@@ -1151,19 +1101,19 @@
     </row>
     <row r="3" spans="1:6" ht="12.75">
       <c r="A3">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F3">
         <v>19</v>
@@ -1171,19 +1121,19 @@
     </row>
     <row r="4" spans="1:6" ht="12.75">
       <c r="A4">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -1198,60 +1148,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="8.421875" widthPt="44.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28125" widthPt="48.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.57421875" widthPt="34.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" widthPt="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.421875" widthPt="49.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28125" widthPt="279.75" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75">
-      <c r="A2">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45636</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-    </row>
+    <row r="1" ht="12.75"/>
   </sheetData>
   <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1269,42 +1172,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="4" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>